<commit_message>
Filtro por tipo operacion ingreso o egreso y documentacion testing del 3 sprint
</commit_message>
<xml_diff>
--- a/Documentation/Testing/Sprint 3/CasosDePrueba_Integrado_Sprint3.xlsx
+++ b/Documentation/Testing/Sprint 3/CasosDePrueba_Integrado_Sprint3.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -146,21 +146,107 @@
   </si>
   <si>
     <t xml:space="preserve">El sistema muestra mensaje de error y redirige a la pantalla de error sin impactar saldo real.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paginación de transacciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la sección Actividad. 
+2. Verificar la cantidad de elementos mostrados. 
+3. Navegar a la siguiente página.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se muestran 10 transacciones por página. El botón de paginación permite navegar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtro por período: Últimos 15 días</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Abrir filtros. 
+2. Seleccionar "Últimos 15 días". 
+3. Aplicar filtros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se muestran solo transacciones dentro de los últimos 15 días.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtro por período: Hoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Abrir filtros. 
+2. Seleccionar "Hoy". 
+3. Aplicar filtros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se muestran sólo las transacciones del día actual.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtro combinado período + tipo operación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar "Última semana" y tipo "Ingresos". 
+2. Aplicar filtros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se muestran sólo ingresos ocurridos en la última semana.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Búsqueda por palabra clave en transacción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar palabra en el campo de búsqueda. 
+2. Presionar Enter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se filtran las transacciones que contengan la palabra ingresada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limpieza de filtros y búsqueda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Aplicar filtros o búsqueda. 
+2. Hacer clic en "Limpiar filtros".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se eliminan todos los filtros y se restablece la vista con todas las transacciones.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -226,17 +312,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -316,233 +414,395 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="85.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="87.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="85.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="87.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="0"/>
+      <c r="H9" s="5" t="n">
+        <v>45942</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="0"/>
+      <c r="H10" s="5" t="n">
+        <v>45942</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="0"/>
+      <c r="H11" s="5" t="n">
+        <v>45942</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="0"/>
+      <c r="H12" s="5" t="n">
+        <v>45942</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="0"/>
+      <c r="H13" s="5" t="n">
+        <v>45942</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="0"/>
+      <c r="H14" s="5" t="n">
+        <v>45942</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>